<commit_message>
Changed ui layout, moved update logic to app
</commit_message>
<xml_diff>
--- a/ui/assets/texts/texts.xlsx
+++ b/ui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9039" uniqueCount="105">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -309,6 +309,29 @@
   </si>
   <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+</t>
   </si>
 </sst>
 </file>
@@ -1776,13 +1799,7 @@
         <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
         <v>77</v>
-      </c>
-      <c r="I3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4">
@@ -1799,15 +1816,15 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -1816,29 +1833,32 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -1853,21 +1873,15 @@
         <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
@@ -1876,89 +1890,32 @@
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>82</v>
-      </c>
-    </row>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
FIX simulator, removed TouchGFX framework from git
</commit_message>
<xml_diff>
--- a/ui/assets/texts/texts.xlsx
+++ b/ui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9039" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8743" uniqueCount="101">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -314,24 +314,10 @@
     <t xml:space="preserve">mi</t>
   </si>
   <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rp</t>
-  </si>
-  <si>
     <t xml:space="preserve">rpm</t>
   </si>
   <si>
-    <t xml:space="preserve">rpm
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">km
-</t>
+    <t xml:space="preserve">SingleUseId8</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1802,7 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5">
@@ -1833,7 +1819,7 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -1878,30 +1864,27 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -1910,7 +1893,7 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10"/>

</xml_diff>

<commit_message>
Changed ui, now there are two analog dials
</commit_message>
<xml_diff>
--- a/ui/assets/texts/texts.xlsx
+++ b/ui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9259" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9421" uniqueCount="107">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1808,129 +1808,81 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>86</v>
+      </c>
+      <c r="G4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>106</v>
-      </c>
-    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
     <row r="11"/>
     <row r="12"/>
   </sheetData>

</xml_diff>

<commit_message>
Updated gui for better visibility
A tenths of km digit was added, proper legends put into dials,
increased font size for current and temperature and added
battery icon
</commit_message>
<xml_diff>
--- a/ui/assets/texts/texts.xlsx
+++ b/ui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13980" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15238" uniqueCount="140">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;text&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partialDis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partialDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;numNew Text</t>
   </si>
 </sst>
 </file>
@@ -1952,7 +1964,7 @@
         <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>102</v>
@@ -1969,7 +1981,7 @@
         <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>102</v>
@@ -1986,7 +1998,7 @@
         <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>102</v>
@@ -2012,7 +2024,7 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -2029,7 +2041,7 @@
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -2047,6 +2059,43 @@
       </c>
       <c r="F12" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: Battery voltage display
</commit_message>
<xml_diff>
--- a/ui/assets/texts/texts.xlsx
+++ b/ui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15238" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19757" uniqueCount="161">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -435,6 +435,69 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;numNew Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batteryVol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batteryVoltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;number&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;text&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,.-s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,.-.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-9,.-.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x39</t>
   </si>
 </sst>
 </file>
@@ -1789,6 +1852,26 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8"/>
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1901,16 +1984,13 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>83</v>
@@ -1920,9 +2000,6 @@
       </c>
       <c r="F4" t="s">
         <v>86</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5">
@@ -2083,7 +2160,7 @@
         <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
@@ -2094,10 +2171,42 @@
       <c r="F14" t="s">
         <v>86</v>
       </c>
-      <c r="G14" t="s">
-        <v>39</v>
-      </c>
-    </row>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>